<commit_message>
light up 4 digit-tubes!!!
</commit_message>
<xml_diff>
--- a/single_cycle/design/instructions.xlsx
+++ b/single_cycle/design/instructions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="122">
   <si>
     <t>instruction</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -473,6 +473,22 @@
   </si>
   <si>
     <t>10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ori</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0d</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>11</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -604,7 +620,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -667,6 +683,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -948,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1672,62 +1691,60 @@
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="7" customFormat="1">
-      <c r="A17" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="6">
-        <v>0</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="6">
-        <v>0</v>
-      </c>
-      <c r="E17" s="6">
-        <v>1</v>
-      </c>
-      <c r="F17" s="6">
-        <v>1</v>
-      </c>
-      <c r="G17" s="6">
-        <v>0</v>
-      </c>
-      <c r="H17" s="6">
-        <v>0</v>
-      </c>
-      <c r="I17" s="6">
-        <v>0</v>
-      </c>
-      <c r="J17" s="6">
-        <v>1</v>
-      </c>
-      <c r="K17" s="6">
-        <v>0</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="N17" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="O17" s="13" t="s">
-        <v>108</v>
+    <row r="17" spans="1:15" s="21" customFormat="1">
+      <c r="A17" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14">
+        <v>0</v>
+      </c>
+      <c r="E17" s="14">
+        <v>1</v>
+      </c>
+      <c r="F17" s="14">
+        <v>0</v>
+      </c>
+      <c r="G17" s="14">
+        <v>0</v>
+      </c>
+      <c r="H17" s="14">
+        <v>0</v>
+      </c>
+      <c r="I17" s="14">
+        <v>0</v>
+      </c>
+      <c r="J17" s="14">
+        <v>0</v>
+      </c>
+      <c r="K17" s="14">
+        <v>1</v>
+      </c>
+      <c r="L17" s="14">
+        <v>0</v>
+      </c>
+      <c r="M17" s="14">
+        <v>0</v>
+      </c>
+      <c r="N17" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="O17" s="15" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:15" s="7" customFormat="1">
       <c r="A18" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="6">
         <v>0</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D18" s="6">
         <v>0</v>
@@ -1754,27 +1771,27 @@
         <v>0</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="M18" s="6" t="s">
         <v>69</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O18" s="13" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:15" s="7" customFormat="1">
       <c r="A19" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="6">
         <v>0</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D19" s="6">
         <v>0</v>
@@ -1801,27 +1818,27 @@
         <v>0</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O19" s="13" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:15" s="7" customFormat="1">
       <c r="A20" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="6">
         <v>0</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D20" s="6">
         <v>0</v>
@@ -1842,74 +1859,77 @@
         <v>0</v>
       </c>
       <c r="J20" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="6">
         <v>0</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O20" s="13" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
-      <c r="A21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="1">
-        <v>0</v>
-      </c>
-      <c r="E21" s="1">
-        <v>1</v>
-      </c>
-      <c r="F21" s="1">
-        <v>0</v>
-      </c>
-      <c r="G21" s="1">
-        <v>0</v>
-      </c>
-      <c r="H21" s="1">
-        <v>0</v>
-      </c>
-      <c r="I21" s="1">
-        <v>0</v>
-      </c>
-      <c r="J21" s="1">
-        <v>0</v>
-      </c>
-      <c r="K21" s="1">
-        <v>1</v>
-      </c>
-      <c r="L21" s="1">
-        <v>1</v>
-      </c>
-      <c r="M21" s="1">
-        <v>0</v>
-      </c>
-      <c r="N21" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="O21" s="8" t="s">
-        <v>109</v>
+    <row r="21" spans="1:15" s="7" customFormat="1">
+      <c r="A21" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0</v>
+      </c>
+      <c r="E21" s="6">
+        <v>1</v>
+      </c>
+      <c r="F21" s="6">
+        <v>1</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0</v>
+      </c>
+      <c r="H21" s="6">
+        <v>0</v>
+      </c>
+      <c r="I21" s="6">
+        <v>0</v>
+      </c>
+      <c r="J21" s="6">
+        <v>0</v>
+      </c>
+      <c r="K21" s="6">
+        <v>0</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="N21" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="O21" s="13" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
@@ -1936,7 +1956,7 @@
         <v>1</v>
       </c>
       <c r="L22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M22" s="1">
         <v>0</v>
@@ -1945,24 +1965,24 @@
         <v>95</v>
       </c>
       <c r="O22" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:15">
       <c r="A23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" s="1">
-        <v>0</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>69</v>
+        <v>1</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
       </c>
       <c r="G23" s="1">
         <v>0</v>
@@ -1970,34 +1990,34 @@
       <c r="H23" s="1">
         <v>0</v>
       </c>
-      <c r="I23" s="1" t="s">
-        <v>72</v>
+      <c r="I23" s="1">
+        <v>0</v>
       </c>
       <c r="J23" s="1">
         <v>0</v>
       </c>
       <c r="K23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M23" s="1">
         <v>0</v>
       </c>
-      <c r="N23" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="O23" s="19" t="s">
-        <v>113</v>
+      <c r="N23" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="O23" s="8" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:15">
       <c r="A24" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>
@@ -2029,19 +2049,19 @@
       <c r="M24" s="1">
         <v>0</v>
       </c>
-      <c r="N24" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="O24" s="8" t="s">
-        <v>111</v>
+      <c r="N24" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="O24" s="19" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:15">
       <c r="A25" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
@@ -2074,18 +2094,18 @@
         <v>0</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O25" s="8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
@@ -2118,18 +2138,18 @@
         <v>0</v>
       </c>
       <c r="N26" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O26" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D27" s="1">
         <v>1</v>
@@ -2162,27 +2182,27 @@
         <v>0</v>
       </c>
       <c r="N27" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O27" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D28" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G28" s="1">
         <v>0</v>
@@ -2193,40 +2213,40 @@
       <c r="I28" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>69</v>
+      <c r="J28" s="1">
+        <v>0</v>
+      </c>
+      <c r="K28" s="1">
+        <v>0</v>
+      </c>
+      <c r="L28" s="1">
+        <v>1</v>
+      </c>
+      <c r="M28" s="1">
+        <v>0</v>
       </c>
       <c r="N28" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O28" s="8" t="s">
-        <v>69</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D29" s="1">
         <v>2</v>
       </c>
       <c r="E29" s="1">
-        <v>1</v>
-      </c>
-      <c r="F29" s="1">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="G29" s="1">
         <v>0</v>
@@ -2234,17 +2254,17 @@
       <c r="H29" s="1">
         <v>0</v>
       </c>
-      <c r="I29" s="1">
-        <v>2</v>
+      <c r="I29" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>69</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M29" s="1" t="s">
         <v>69</v>
@@ -2253,74 +2273,71 @@
         <v>101</v>
       </c>
       <c r="O29" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="1">
+        <v>2</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1">
+        <v>2</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+      <c r="I30" s="1">
+        <v>2</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N30" s="9" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" s="7" customFormat="1">
-      <c r="A30" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="6">
-        <v>0</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D30" s="6">
-        <v>3</v>
-      </c>
-      <c r="E30" s="6">
-        <v>0</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G30" s="6">
-        <v>0</v>
-      </c>
-      <c r="H30" s="6">
-        <v>0</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="K30" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="L30" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="M30" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="N30" s="12" t="s">
+      <c r="O30" s="8" t="s">
         <v>101</v>
-      </c>
-      <c r="O30" s="13" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:15" s="7" customFormat="1">
       <c r="A31" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="6">
         <v>0</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D31" s="6">
         <v>3</v>
       </c>
       <c r="E31" s="6">
-        <v>1</v>
-      </c>
-      <c r="F31" s="6">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="G31" s="6">
         <v>0</v>
@@ -2328,17 +2345,17 @@
       <c r="H31" s="6">
         <v>0</v>
       </c>
-      <c r="I31" s="6">
-        <v>2</v>
+      <c r="I31" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M31" s="6" t="s">
         <v>69</v>
@@ -2347,37 +2364,84 @@
         <v>101</v>
       </c>
       <c r="O31" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" s="7" customFormat="1">
+      <c r="A32" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="6">
+        <v>0</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="6">
+        <v>3</v>
+      </c>
+      <c r="E32" s="6">
+        <v>1</v>
+      </c>
+      <c r="F32" s="6">
+        <v>1</v>
+      </c>
+      <c r="G32" s="6">
+        <v>0</v>
+      </c>
+      <c r="H32" s="6">
+        <v>0</v>
+      </c>
+      <c r="I32" s="6">
+        <v>2</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="L32" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="N32" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="O32" s="13" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:15" s="5" customFormat="1">
-      <c r="A32" s="3" t="s">
+    <row r="33" spans="1:15" s="5" customFormat="1">
+      <c r="A33" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4">
-        <v>1</v>
-      </c>
-      <c r="F32" s="4">
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4">
+        <v>1</v>
+      </c>
+      <c r="F33" s="4">
         <v>3</v>
       </c>
-      <c r="G32" s="4">
-        <v>0</v>
-      </c>
-      <c r="H32" s="4">
-        <v>0</v>
-      </c>
-      <c r="I32" s="4">
+      <c r="G33" s="4">
+        <v>0</v>
+      </c>
+      <c r="H33" s="4">
+        <v>0</v>
+      </c>
+      <c r="I33" s="4">
         <v>2</v>
       </c>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="15"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>